<commit_message>
Added VendorID to all types of Products
</commit_message>
<xml_diff>
--- a/DBStructure-Example.xlsx
+++ b/DBStructure-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5400" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5400" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="2" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="CharacterClasses" sheetId="5" r:id="rId4"/>
     <sheet name="Accounts" sheetId="7" r:id="rId5"/>
     <sheet name="Vendors" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
-    <sheet name="Resources" sheetId="8" r:id="rId8"/>
-    <sheet name="ResourceTypes" sheetId="9" r:id="rId9"/>
+    <sheet name="Resources" sheetId="8" r:id="rId7"/>
+    <sheet name="ResourceTypes" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -1087,7 +1087,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="A1:H16"/>
+      <selection activeCell="C2" sqref="C2:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2253,23 +2253,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="2" width="10.85546875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" customHeight="1">
+    <row r="1" spans="1:6" ht="32.25" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>113</v>
       </c>
@@ -2277,269 +2277,315 @@
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5" ht="42.75" customHeight="1">
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="42.75" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23">
+        <v>9</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="23">
+      <c r="D3" s="23">
         <v>12</v>
       </c>
-      <c r="D3" s="28">
+      <c r="E3" s="28">
         <v>0.68</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="23">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="23">
+        <v>10</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="23">
+      <c r="D4" s="23">
         <v>13</v>
       </c>
-      <c r="D4" s="28">
+      <c r="E4" s="28">
         <v>1.68</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="23">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23">
+        <v>11</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="23">
+      <c r="D5" s="23">
         <v>14</v>
       </c>
-      <c r="D5" s="28">
+      <c r="E5" s="28">
         <v>2.68</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="23">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="23">
+        <v>12</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="23">
+      <c r="D6" s="23">
         <v>15</v>
       </c>
-      <c r="D6" s="28">
+      <c r="E6" s="28">
         <v>3.68</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="23">
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="23">
+        <v>13</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="23">
+      <c r="D7" s="23">
         <v>16</v>
       </c>
-      <c r="D7" s="28">
+      <c r="E7" s="28">
         <v>4.68</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="23">
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="23">
+        <v>14</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="23">
+      <c r="D8" s="23">
         <v>17</v>
       </c>
-      <c r="D8" s="28">
+      <c r="E8" s="28">
         <v>5.68</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="F8" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="23">
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="23">
+        <v>15</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="23">
+      <c r="D9" s="23">
         <v>18</v>
       </c>
-      <c r="D9" s="28">
+      <c r="E9" s="28">
         <v>6.68</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="F9" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="23">
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="23">
+        <v>16</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="23">
+      <c r="D10" s="23">
         <v>19</v>
       </c>
-      <c r="D10" s="28">
+      <c r="E10" s="28">
         <v>7.68</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="F10" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="23">
         <v>9</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="23">
+        <v>17</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="23">
+      <c r="D11" s="23">
         <v>20</v>
       </c>
-      <c r="D11" s="28">
+      <c r="E11" s="28">
         <v>8.68</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="F11" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="23">
         <v>10</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="23">
+        <v>18</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="23">
+      <c r="D12" s="23">
         <v>21</v>
       </c>
-      <c r="D12" s="28">
+      <c r="E12" s="28">
         <v>9.68</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="F12" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="23">
         <v>11</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23">
+        <v>19</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="23">
+      <c r="D13" s="23">
         <v>22</v>
       </c>
-      <c r="D13" s="28">
+      <c r="E13" s="28">
         <v>10.68</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="23">
         <v>12</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23">
+        <v>20</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="23">
+      <c r="D14" s="23">
         <v>23</v>
       </c>
-      <c r="D14" s="28">
+      <c r="E14" s="28">
         <v>11.68</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="23">
         <v>13</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23">
+        <v>21</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="23">
+      <c r="D15" s="23">
         <v>24</v>
       </c>
-      <c r="D15" s="28">
+      <c r="E15" s="28">
         <v>12.68</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="F15" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="23">
         <v>14</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23">
+        <v>22</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="23">
+      <c r="D16" s="23">
         <v>25</v>
       </c>
-      <c r="D16" s="28">
+      <c r="E16" s="28">
         <v>13.68</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="F16" s="23" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4:B16" r:id="rId2" display="koreanplayer@abv.bg"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4:C16" r:id="rId2" display="koreanplayer@abv.bg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2743,6 +2789,341 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="23" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="23" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="32.25" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:4" ht="42.75" customHeight="1">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23">
+        <v>3</v>
+      </c>
+      <c r="C3" s="23">
+        <v>9</v>
+      </c>
+      <c r="D3" s="23">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="23">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23">
+        <v>2</v>
+      </c>
+      <c r="C4" s="23">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="23">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23">
+        <v>2</v>
+      </c>
+      <c r="C5" s="23">
+        <v>11</v>
+      </c>
+      <c r="D5" s="23">
+        <v>20002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="23">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23">
+        <v>12</v>
+      </c>
+      <c r="D6" s="23">
+        <v>20003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23">
+        <v>13</v>
+      </c>
+      <c r="D7" s="23">
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="23">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23">
+        <v>20005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="23">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23">
+        <v>15</v>
+      </c>
+      <c r="D9" s="23">
+        <v>20006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="23">
+        <v>8</v>
+      </c>
+      <c r="B10" s="23">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23">
+        <v>16</v>
+      </c>
+      <c r="D10" s="23">
+        <v>20007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="23">
+        <v>9</v>
+      </c>
+      <c r="B11" s="23">
+        <v>4</v>
+      </c>
+      <c r="C11" s="23">
+        <v>17</v>
+      </c>
+      <c r="D11" s="23">
+        <v>20008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="23">
+        <v>10</v>
+      </c>
+      <c r="B12" s="23">
+        <v>5</v>
+      </c>
+      <c r="C12" s="23">
+        <v>18</v>
+      </c>
+      <c r="D12" s="23">
+        <v>20009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="23">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23">
+        <v>3</v>
+      </c>
+      <c r="C13" s="23">
+        <v>19</v>
+      </c>
+      <c r="D13" s="23">
+        <v>20010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="23">
+        <v>12</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1</v>
+      </c>
+      <c r="C14" s="23">
+        <v>20</v>
+      </c>
+      <c r="D14" s="23">
+        <v>20011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="23">
+        <v>13</v>
+      </c>
+      <c r="B15" s="23">
+        <v>4</v>
+      </c>
+      <c r="C15" s="23">
+        <v>21</v>
+      </c>
+      <c r="D15" s="23">
+        <v>20012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="23">
+        <v>14</v>
+      </c>
+      <c r="B16" s="23">
+        <v>4</v>
+      </c>
+      <c r="C16" s="23">
+        <v>22</v>
+      </c>
+      <c r="D16" s="23">
+        <v>20013</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="23" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="32.25" customHeight="1">
+      <c r="A1" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="23">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="23">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="23">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="23">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="23">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3097,293 +3478,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="32.25" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" ht="42.75" customHeight="1">
-      <c r="A2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="23">
-        <v>1</v>
-      </c>
-      <c r="B3" s="23">
-        <v>3</v>
-      </c>
-      <c r="C3" s="23">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="23">
-        <v>2</v>
-      </c>
-      <c r="B4" s="23">
-        <v>2</v>
-      </c>
-      <c r="C4" s="23">
-        <v>20001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="23">
-        <v>3</v>
-      </c>
-      <c r="B5" s="23">
-        <v>2</v>
-      </c>
-      <c r="C5" s="23">
-        <v>20002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23">
-        <v>4</v>
-      </c>
-      <c r="B6" s="23">
-        <v>1</v>
-      </c>
-      <c r="C6" s="23">
-        <v>20003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23">
-        <v>5</v>
-      </c>
-      <c r="B7" s="23">
-        <v>2</v>
-      </c>
-      <c r="C7" s="23">
-        <v>20004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23">
-        <v>6</v>
-      </c>
-      <c r="B8" s="23">
-        <v>1</v>
-      </c>
-      <c r="C8" s="23">
-        <v>20005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23">
-        <v>7</v>
-      </c>
-      <c r="B9" s="23">
-        <v>2</v>
-      </c>
-      <c r="C9" s="23">
-        <v>20006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="23">
-        <v>8</v>
-      </c>
-      <c r="B10" s="23">
-        <v>5</v>
-      </c>
-      <c r="C10" s="23">
-        <v>20007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="23">
-        <v>9</v>
-      </c>
-      <c r="B11" s="23">
-        <v>4</v>
-      </c>
-      <c r="C11" s="23">
-        <v>20008</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="23">
-        <v>10</v>
-      </c>
-      <c r="B12" s="23">
-        <v>5</v>
-      </c>
-      <c r="C12" s="23">
-        <v>20009</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="23">
-        <v>11</v>
-      </c>
-      <c r="B13" s="23">
-        <v>3</v>
-      </c>
-      <c r="C13" s="23">
-        <v>20010</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="23">
-        <v>12</v>
-      </c>
-      <c r="B14" s="23">
-        <v>1</v>
-      </c>
-      <c r="C14" s="23">
-        <v>20011</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23">
-        <v>13</v>
-      </c>
-      <c r="B15" s="23">
-        <v>4</v>
-      </c>
-      <c r="C15" s="23">
-        <v>20012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="23">
-        <v>14</v>
-      </c>
-      <c r="B16" s="23">
-        <v>4</v>
-      </c>
-      <c r="C16" s="23">
-        <v>20013</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="23" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="32.25" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="30"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="23">
-        <v>1</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="23">
-        <v>2</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="23">
-        <v>3</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="23">
-        <v>4</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="23">
-        <v>5</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="23">
-        <v>6</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="23">
-        <v>7</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>